<commit_message>
Results 13-3 rolling horizon tuning lambda
</commit_message>
<xml_diff>
--- a/results/summary_table_lambda_tuning.xlsx
+++ b/results/summary_table_lambda_tuning.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\SimPyManufacturing\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{53F15117-DB6B-4543-90C4-AA8C47918885}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A9268A5-73A4-4967-BAD2-E574C094E3AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14790" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -19,10 +19,23 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">summary_table_latest_version_si!$B$1:$Q$81</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="9" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -398,7 +411,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -876,9 +889,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1032,6 +1044,9 @@
       <c:pivotFmt>
         <c:idx val="1"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -2193,7 +2208,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Kim van den Houten" refreshedDate="44998.489303703704" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="82">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Kim van den Houten" refreshedDate="44998.489303703704" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="82" xr:uid="{00000000-000A-0000-FFFF-FFFF09000000}">
   <cacheSource type="worksheet">
     <worksheetSource ref="B1:Q1048576" sheet="summary_table_latest_version_si"/>
   </cacheSource>
@@ -3747,7 +3762,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A3:C12" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="16">
     <pivotField showAll="0"/>
@@ -4155,10 +4170,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="R22" sqref="R22"/>
     </sheetView>
   </sheetViews>
@@ -4170,7 +4185,7 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>115</v>
       </c>
       <c r="B3" t="s">
@@ -4181,101 +4196,101 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>0</v>
-      </c>
-      <c r="B4" s="1">
+      <c r="A4" s="2">
+        <v>0</v>
+      </c>
+      <c r="B4">
         <v>6689</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4">
         <v>8555.2000000000007</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+      <c r="A5" s="2">
         <v>0.01</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5">
         <v>6672.4</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5">
         <v>8587.6</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <v>0.1</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6">
         <v>6676.3</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6">
         <v>8541.7999999999993</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+      <c r="A7" s="2">
         <v>0.25</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7">
         <v>6674.2</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7">
         <v>8586.2999999999993</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+      <c r="A8" s="2">
         <v>0.5</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8">
         <v>6670.5</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8">
         <v>8570.7999999999993</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
+      <c r="A9" s="2">
         <v>0.9</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9">
         <v>6663.3</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9">
         <v>8659.4</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
+      <c r="A10" s="2">
         <v>0.99</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10">
         <v>6661.1</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10">
         <v>8919.2000000000007</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
-        <v>1</v>
-      </c>
-      <c r="B11" s="1">
+      <c r="A11" s="2">
+        <v>1</v>
+      </c>
+      <c r="B11">
         <v>6666.8</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11">
         <v>13371</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12">
         <v>6671.7</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12">
         <v>9223.9125000000004</v>
       </c>
     </row>
@@ -4286,16 +4301,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:L1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="6" max="6" width="31" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8669,7 +8685,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:Q81">
+  <autoFilter ref="B1:Q81" xr:uid="{00000000-0009-0000-0000-000001000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:Q81">
       <sortCondition ref="F1:F81"/>
     </sortState>

</xml_diff>